<commit_message>
Se realizaron ejercicios del bloque 4 y unos del bloque 3
</commit_message>
<xml_diff>
--- a/Bloque 3/Analisis de problemas.xlsx
+++ b/Bloque 3/Analisis de problemas.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Documents\proyectosdegit\Clasesdec\Clases_De_C\Bloque 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8623793-1CB2-457A-8500-70E6BBDA1BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24728E8E-7AA6-4370-B5AA-AB9B33A6CC97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{89236BF2-72C1-4065-9A25-0142C639815A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{89236BF2-72C1-4065-9A25-0142C639815A}"/>
   </bookViews>
   <sheets>
     <sheet name="PS3_19" sheetId="1" r:id="rId1"/>
     <sheet name="PS3_20" sheetId="2" r:id="rId2"/>
     <sheet name="PS3_14" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
+    <sheet name="Variable_problema2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1596,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40061183-F35E-4973-B283-236D1E85EF39}">
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1712,7 +1712,7 @@
         <v>195.73333333333335</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="E2:K2" si="0">E2+POWER(-1,F1+1)*POWER($A$2,2*F1-1)/FACT(2*F1-1)</f>
+        <f t="shared" ref="F2:K2" si="0">E2+POWER(-1,F1+1)*POWER($A$2,2*F1-1)/FACT(2*F1-1)</f>
         <v>-220.36825396825395</v>
       </c>
       <c r="G2">
@@ -2184,7 +2184,7 @@
         <v>108.66666666666666</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:S19" si="18">ABS(F12)-ABS(E12)</f>
+        <f t="shared" ref="F19:R19" si="18">ABS(F12)-ABS(E12)</f>
         <v>84.755555555555588</v>
       </c>
       <c r="G19">
@@ -2247,12 +2247,168 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E297ADE-2ACD-4035-8878-DFAB3F4FD2F2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <f>MOD(A1,10)</f>
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <f>ROUNDDOWN(A1/10,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <f>MOD(A2,10)</f>
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>ROUNDDOWN(A2/10,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>MOD(C2,10)</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>ROUNDDOWN(C2/10,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>105</v>
+      </c>
+      <c r="B3" s="1">
+        <f>MOD(A3,10)</f>
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <f>ROUNDDOWN(A3/10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <f>MOD(C3,10)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>ROUNDDOWN(C3/10,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>MOD(E3,10)</f>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f>ROUNDDOWN(E3/10,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4567</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f>ROUNDDOWN(MOD($A$8,POWER(10,4)),0)</f>
+        <v>4567</v>
+      </c>
+      <c r="E8">
+        <f>ROUNDDOWN(MOD($A$8,POWER(10,2-1)),0)</f>
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="E8:G8" si="0">ROUNDDOWN(MOD($A$8,POWER(10,4-1)),0)</f>
+        <v>567</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>567</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f>ROUNDDOWN($A$8/POWER(10,4-1),0)</f>
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f>ROUNDDOWN(MOD(D11,10),0)</f>
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <f>ROUNDDOWN($A$8/POWER(10,3-1),0)</f>
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <f>ROUNDDOWN(MOD(F11,10),0)</f>
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <f>ROUNDDOWN($A$8/POWER(10,2-1),0)</f>
+        <v>456</v>
+      </c>
+      <c r="I11">
+        <f>ROUNDDOWN(MOD(H11,10),0)</f>
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <f>$A$8</f>
+        <v>4567</v>
+      </c>
+      <c r="K11">
+        <f>ROUNDDOWN(MOD(J11,10),0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <f>4*1</f>
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <f>4+5*10</f>
+        <v>54</v>
+      </c>
+      <c r="I13">
+        <f>54+6*100</f>
+        <v>654</v>
+      </c>
+      <c r="K13">
+        <f>654+7*1000</f>
+        <v>7654</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregaron los hipervinculos de los anexos
</commit_message>
<xml_diff>
--- a/Bloque 3/Analisis de problemas.xlsx
+++ b/Bloque 3/Analisis de problemas.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Documents\proyectosdegit\Clasesdec\Clases_De_C\Bloque 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24728E8E-7AA6-4370-B5AA-AB9B33A6CC97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9259D465-7D32-49B9-A030-A6B9C607F528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{89236BF2-72C1-4065-9A25-0142C639815A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{89236BF2-72C1-4065-9A25-0142C639815A}"/>
   </bookViews>
   <sheets>
     <sheet name="PS3_19" sheetId="1" r:id="rId1"/>
     <sheet name="PS3_20" sheetId="2" r:id="rId2"/>
     <sheet name="PS3_14" sheetId="3" r:id="rId3"/>
     <sheet name="Variable_problema2" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2249,7 +2250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E297ADE-2ACD-4035-8878-DFAB3F4FD2F2}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -2348,7 +2349,7 @@
         <v>7</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="E8:G8" si="0">ROUNDDOWN(MOD($A$8,POWER(10,4-1)),0)</f>
+        <f t="shared" ref="F8:G8" si="0">ROUNDDOWN(MOD($A$8,POWER(10,4-1)),0)</f>
         <v>567</v>
       </c>
       <c r="G8">
@@ -2411,4 +2412,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB87A16A-E543-479F-A23F-67C74695630C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se finalizaron los problemas del bloque 5, solo el 11 no lo pude hacer
</commit_message>
<xml_diff>
--- a/Bloque 3/Analisis de problemas.xlsx
+++ b/Bloque 3/Analisis de problemas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Documents\proyectosdegit\Clasesdec\Clases_De_C\Bloque 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9259D465-7D32-49B9-A030-A6B9C607F528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D813DF5-B291-444D-86DE-F82881097827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{89236BF2-72C1-4065-9A25-0142C639815A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="PS3_20" sheetId="2" r:id="rId2"/>
     <sheet name="PS3_14" sheetId="3" r:id="rId3"/>
     <sheet name="Variable_problema2" sheetId="4" r:id="rId4"/>
-    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
+    <sheet name="matriz_inversa" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="22">
   <si>
     <t>i</t>
   </si>
@@ -64,6 +64,45 @@
   </si>
   <si>
     <t>Coseno(x)</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>2,0</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>col+1</t>
+  </si>
+  <si>
+    <t>col+2</t>
+  </si>
+  <si>
+    <t>fila+1</t>
+  </si>
+  <si>
+    <t>flia+2</t>
   </si>
 </sst>
 </file>
@@ -96,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -113,17 +152,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,6 +195,303 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{555E522F-335C-471C-A6B6-0EA0FC5611A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4922520" y="876300"/>
+          <a:ext cx="5463540" cy="4587240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>mat_aux[][]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>mat[][]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>for(i=0;i&lt;fil;i++){</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>   for(j=0;j&lt;col;j++){</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>      if(i==0||i==2){</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>        </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>for(k=0;k&lt;fil-1;k++){</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>           for(l=0;l&lt;col-1;l++){</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>              if(j==0||j==2)</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>              mat_aux[k][l]=mat[i+1+k][(j+1+l)%3];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>              else</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>               </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>mat_aux[k][l]=mat[i+1+k][(j*2+l*2+1)%3];</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>             }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>           }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>         }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>       else{</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>         </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>if(j==0||j==2)</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>              mat_aux[k][l]=mat[[(i*2+k*2+1)%3][(j+1+l)%3];</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>              else</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>               mat_aux[k][l]=mat[(i*2+k*2+1)%3][(j*2+l*2+1)%3];</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>        }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t>     }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t> }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2416,12 +2769,201 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB87A16A-E543-479F-A23F-67C74695630C}">
-  <dimension ref="A1"/>
+  <dimension ref="B5:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>